<commit_message>
dynamic scenarios for batch and program added
</commit_message>
<xml_diff>
--- a/7CRUDCarriers_LMS_API/src/test/resources/excelData/batch_testdata.xlsx
+++ b/7CRUDCarriers_LMS_API/src/test/resources/excelData/batch_testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavit\git\7CRUDCarriers_LMS_API\7CRUDCarriers_LMS_API\src\test\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC41591-337E-450B-B8C6-9327FAC2E213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44BA897-8DD9-4344-8885-DEE96E75534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>StatusCode</t>
-  </si>
-  <si>
-    <t>Jan23-CRUDCarriers-SDET-519</t>
   </si>
   <si>
     <t>Body</t>
@@ -321,8 +318,11 @@
     <t>Update batch with valid BatchId and without JSON Schema</t>
   </si>
   <si>
+    <t>Jan23-CRUDCarriers-SDET-011</t>
+  </si>
+  <si>
     <t xml:space="preserve"> {
-    "batchName":"Jan23-CRUDCarriers-SDET-2530",
+    "batchName":"Jan23-CRUDCarriers-SDET-3531",
     "batchDescription":"API Testing",
     "batchStatus":"Active",
     "batchNoOfClasses":"12",
@@ -331,7 +331,7 @@
   </si>
   <si>
     <t xml:space="preserve"> {
-    "batchName":"46546464-30",
+    "batchName":"46546464-31",
     "batchDescription":"4556",
     "batchStatus":"1234",
     "batchNoOfClasses":"12",
@@ -340,7 +340,7 @@
   </si>
   <si>
     <t>{
-    "batchName":"Jan23-CRUDCarriers-SDET-2531",
+    "batchName":"Jan23-CRUDCarriers-SDET-3231",
     "batchDescription":"API Testing",
     "batchStatus":"Active",
     "batchNoOfClasses":"21",
@@ -352,11 +352,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -547,98 +554,98 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -883,7 +890,7 @@
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3">
@@ -892,10 +899,10 @@
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4">
-        <v>1588</v>
+        <v>5413</v>
       </c>
       <c r="C3" s="3">
         <v>200</v>
@@ -903,7 +910,7 @@
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4">
         <v>10</v>
@@ -914,10 +921,10 @@
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3">
         <v>400</v>
@@ -925,7 +932,7 @@
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3">
@@ -934,7 +941,7 @@
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4">
         <v>45.36</v>
@@ -945,7 +952,7 @@
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4">
         <v>305</v>
@@ -956,10 +963,10 @@
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>3</v>
+        <v>29</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>71</v>
       </c>
       <c r="C9" s="3">
         <v>200</v>
@@ -967,7 +974,7 @@
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="4">
         <v>105</v>
@@ -978,10 +985,10 @@
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3">
         <v>400</v>
@@ -989,7 +996,7 @@
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="3">
@@ -3934,7 +3941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D999"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3952,18 +3959,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>72</v>
@@ -3972,54 +3979,54 @@
         <v>201</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>73</v>
@@ -4028,133 +4035,133 @@
         <v>201</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="7">
         <v>400</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4">
         <v>400</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4">
         <v>400</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="33" t="s">
         <v>74</v>
       </c>
       <c r="C15" s="4">
         <v>201</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7120,7 +7127,7 @@
   <dimension ref="A1:E995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7141,118 +7148,118 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="24">
         <v>898</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="25">
         <v>609999</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="26">
         <v>400</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="26">
         <v>400</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="30">
         <v>405</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="28">
         <v>609.1</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="30">
         <v>400</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="28">
         <v>-609</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="30">
         <v>400</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="28">
         <v>609</v>
@@ -7262,7 +7269,7 @@
         <v>415</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7281,107 +7288,107 @@
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="24">
+        <v>5413</v>
+      </c>
+      <c r="C11" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="24">
-        <v>898</v>
-      </c>
-      <c r="C11" s="33" t="s">
+      <c r="D11" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="25">
         <v>609999</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="26">
         <v>400</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="26">
         <v>400</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="30">
         <v>405</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="28">
         <v>609.1</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="30">
         <v>400</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="28">
         <v>-609</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="30">
         <v>400</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="28">
         <v>609</v>
@@ -7391,7 +7398,7 @@
         <v>415</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8437,7 +8444,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8457,26 +8464,26 @@
         <v>2</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="19">
-        <v>264</v>
+        <v>2409</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="19">
         <v>1234</v>
@@ -8485,47 +8492,47 @@
         <v>400</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19">
         <v>405</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="19">
         <v>400</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="C6" s="19">
         <v>400</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/Pavithra-kamat/7CRUDCarriers_LMS_API"
This reverts commit 8b3cde0601a401d30bbaf79ca97cc74a8718cc6a, reversing
changes made to f4a3d5b7b56db02ff1d64a00bf714e5b9d4952e5.
</commit_message>
<xml_diff>
--- a/7CRUDCarriers_LMS_API/src/test/resources/excelData/batch_testdata.xlsx
+++ b/7CRUDCarriers_LMS_API/src/test/resources/excelData/batch_testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavit\git\7CRUDCarriers_LMS_API\7CRUDCarriers_LMS_API\src\test\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44BA897-8DD9-4344-8885-DEE96E75534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC41591-337E-450B-B8C6-9327FAC2E213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>StatusCode</t>
+  </si>
+  <si>
+    <t>Jan23-CRUDCarriers-SDET-519</t>
   </si>
   <si>
     <t>Body</t>
@@ -318,11 +321,8 @@
     <t>Update batch with valid BatchId and without JSON Schema</t>
   </si>
   <si>
-    <t>Jan23-CRUDCarriers-SDET-011</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {
-    "batchName":"Jan23-CRUDCarriers-SDET-3531",
+    "batchName":"Jan23-CRUDCarriers-SDET-2530",
     "batchDescription":"API Testing",
     "batchStatus":"Active",
     "batchNoOfClasses":"12",
@@ -331,7 +331,7 @@
   </si>
   <si>
     <t xml:space="preserve"> {
-    "batchName":"46546464-31",
+    "batchName":"46546464-30",
     "batchDescription":"4556",
     "batchStatus":"1234",
     "batchNoOfClasses":"12",
@@ -340,7 +340,7 @@
   </si>
   <si>
     <t>{
-    "batchName":"Jan23-CRUDCarriers-SDET-3231",
+    "batchName":"Jan23-CRUDCarriers-SDET-2531",
     "batchDescription":"API Testing",
     "batchStatus":"Active",
     "batchNoOfClasses":"21",
@@ -352,18 +352,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -554,98 +547,98 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -890,7 +883,7 @@
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3">
@@ -899,10 +892,10 @@
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4">
-        <v>5413</v>
+        <v>1588</v>
       </c>
       <c r="C3" s="3">
         <v>200</v>
@@ -910,7 +903,7 @@
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4">
         <v>10</v>
@@ -921,10 +914,10 @@
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="C5" s="3">
         <v>400</v>
@@ -932,7 +925,7 @@
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3">
@@ -941,7 +934,7 @@
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4">
         <v>45.36</v>
@@ -952,7 +945,7 @@
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="4">
         <v>305</v>
@@ -963,10 +956,10 @@
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>71</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>3</v>
       </c>
       <c r="C9" s="3">
         <v>200</v>
@@ -974,7 +967,7 @@
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="4">
         <v>105</v>
@@ -985,10 +978,10 @@
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3">
         <v>400</v>
@@ -996,7 +989,7 @@
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="3">
@@ -3941,7 +3934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D999"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3959,18 +3952,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>72</v>
@@ -3979,54 +3972,54 @@
         <v>201</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>73</v>
@@ -4035,133 +4028,133 @@
         <v>201</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7">
         <v>400</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4">
         <v>400</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="4">
         <v>400</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="32" t="s">
         <v>74</v>
       </c>
       <c r="C15" s="4">
         <v>201</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7127,7 +7120,7 @@
   <dimension ref="A1:E995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7148,118 +7141,118 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" s="24">
         <v>898</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" s="25">
         <v>609999</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="26">
         <v>400</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D4" s="26">
         <v>400</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5" s="30">
         <v>405</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="28">
         <v>609.1</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6" s="30">
         <v>400</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" s="28">
         <v>-609</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D7" s="30">
         <v>400</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B8" s="28">
         <v>609</v>
@@ -7269,7 +7262,7 @@
         <v>415</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7288,107 +7281,107 @@
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B11" s="24">
-        <v>5413</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>62</v>
+        <v>898</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="25">
         <v>609999</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="26">
         <v>400</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D13" s="26">
         <v>400</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="30">
         <v>405</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B15" s="28">
         <v>609.1</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="30">
         <v>400</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" s="28">
         <v>-609</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="30">
         <v>400</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B17" s="28">
         <v>609</v>
@@ -7398,7 +7391,7 @@
         <v>415</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8444,7 +8437,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8464,26 +8457,26 @@
         <v>2</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="19">
-        <v>2409</v>
+        <v>264</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="19">
         <v>1234</v>
@@ -8492,47 +8485,47 @@
         <v>400</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19">
         <v>405</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="19">
         <v>400</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C6" s="19">
         <v>400</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/Pavithra-kamat/7CRUDCarriers_LMS_API""
This reverts commit 3f93395852238dbb20702e4fd0514eda110bc8bc.
</commit_message>
<xml_diff>
--- a/7CRUDCarriers_LMS_API/src/test/resources/excelData/batch_testdata.xlsx
+++ b/7CRUDCarriers_LMS_API/src/test/resources/excelData/batch_testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavit\git\7CRUDCarriers_LMS_API\7CRUDCarriers_LMS_API\src\test\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC41591-337E-450B-B8C6-9327FAC2E213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44BA897-8DD9-4344-8885-DEE96E75534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>StatusCode</t>
-  </si>
-  <si>
-    <t>Jan23-CRUDCarriers-SDET-519</t>
   </si>
   <si>
     <t>Body</t>
@@ -321,8 +318,11 @@
     <t>Update batch with valid BatchId and without JSON Schema</t>
   </si>
   <si>
+    <t>Jan23-CRUDCarriers-SDET-011</t>
+  </si>
+  <si>
     <t xml:space="preserve"> {
-    "batchName":"Jan23-CRUDCarriers-SDET-2530",
+    "batchName":"Jan23-CRUDCarriers-SDET-3531",
     "batchDescription":"API Testing",
     "batchStatus":"Active",
     "batchNoOfClasses":"12",
@@ -331,7 +331,7 @@
   </si>
   <si>
     <t xml:space="preserve"> {
-    "batchName":"46546464-30",
+    "batchName":"46546464-31",
     "batchDescription":"4556",
     "batchStatus":"1234",
     "batchNoOfClasses":"12",
@@ -340,7 +340,7 @@
   </si>
   <si>
     <t>{
-    "batchName":"Jan23-CRUDCarriers-SDET-2531",
+    "batchName":"Jan23-CRUDCarriers-SDET-3231",
     "batchDescription":"API Testing",
     "batchStatus":"Active",
     "batchNoOfClasses":"21",
@@ -352,11 +352,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -547,98 +554,98 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -883,7 +890,7 @@
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3">
@@ -892,10 +899,10 @@
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4">
-        <v>1588</v>
+        <v>5413</v>
       </c>
       <c r="C3" s="3">
         <v>200</v>
@@ -903,7 +910,7 @@
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4">
         <v>10</v>
@@ -914,10 +921,10 @@
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3">
         <v>400</v>
@@ -925,7 +932,7 @@
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3">
@@ -934,7 +941,7 @@
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4">
         <v>45.36</v>
@@ -945,7 +952,7 @@
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4">
         <v>305</v>
@@ -956,10 +963,10 @@
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>3</v>
+        <v>29</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>71</v>
       </c>
       <c r="C9" s="3">
         <v>200</v>
@@ -967,7 +974,7 @@
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="4">
         <v>105</v>
@@ -978,10 +985,10 @@
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3">
         <v>400</v>
@@ -989,7 +996,7 @@
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="3">
@@ -3934,7 +3941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D999"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3952,18 +3959,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>72</v>
@@ -3972,54 +3979,54 @@
         <v>201</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>73</v>
@@ -4028,133 +4035,133 @@
         <v>201</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="7">
         <v>400</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4">
         <v>400</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4">
         <v>400</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="33" t="s">
         <v>74</v>
       </c>
       <c r="C15" s="4">
         <v>201</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7120,7 +7127,7 @@
   <dimension ref="A1:E995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7141,118 +7148,118 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="24">
         <v>898</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="25">
         <v>609999</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="26">
         <v>400</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="26">
         <v>400</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="30">
         <v>405</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="28">
         <v>609.1</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="30">
         <v>400</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="28">
         <v>-609</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="30">
         <v>400</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="28">
         <v>609</v>
@@ -7262,7 +7269,7 @@
         <v>415</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7281,107 +7288,107 @@
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="24">
+        <v>5413</v>
+      </c>
+      <c r="C11" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="24">
-        <v>898</v>
-      </c>
-      <c r="C11" s="33" t="s">
+      <c r="D11" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="25">
         <v>609999</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="26">
         <v>400</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="26">
         <v>400</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="30">
         <v>405</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="28">
         <v>609.1</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="30">
         <v>400</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="28">
         <v>-609</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="30">
         <v>400</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="28">
         <v>609</v>
@@ -7391,7 +7398,7 @@
         <v>415</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8437,7 +8444,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8457,26 +8464,26 @@
         <v>2</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="19">
-        <v>264</v>
+        <v>2409</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="19">
         <v>1234</v>
@@ -8485,47 +8492,47 @@
         <v>400</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19">
         <v>405</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="19">
         <v>400</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="C6" s="19">
         <v>400</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>